<commit_message>
end to end works  + cdp done + pdp done + sdp done (conv left to fullly complete)
</commit_message>
<xml_diff>
--- a/all_funcs_to_excel/all_regs_with_params_2.xlsx
+++ b/all_funcs_to_excel/all_regs_with_params_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasdhome/Documents/thomas/Princeton/Fall 2022-2023/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB2DE35-CC87-F44D-A30C-7E5CD5A7FA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208082C0-69D5-F64B-BA17-72A5EBC4E8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="520" windowWidth="29720" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2840" yWindow="520" windowWidth="30760" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3418" uniqueCount="1933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3419" uniqueCount="1934">
   <si>
     <t>Core</t>
   </si>
@@ -5472,22 +5472,6 @@
 NVDLA_PDP_PARTIAL_WIDTH_OUT_MID (20-29) = 0 (unused)</t>
   </si>
   <si>
-    <t>NVDLA_PDP_KERNEL_WIDTH (0-3) = pool_size, 
-NVDLA_PDP_KERNEL_HEIGHT (8-11) = pool_size, 
-NVDLA_PDP_KERNEL_STRIDE_WIDTH (16-19) = strides[1], 
-NVDLA_PDP_KERNEL_STRIDE_HEIGHT (20-23) = strides[0]</t>
-  </si>
-  <si>
-    <t>NVDLA_PDP_RDMA_KERNEL_WIDTH (0-3) = weight width (from c++ driver), 
-NVDLA_PDP_RDMA_KERNEL_STRIDE_WIDTH (4-7) = strides[1]</t>
-  </si>
-  <si>
-    <t>NVDLA_PDP_RECIP_KERNEL_WIDTH (0-16) = 2^16 / pool_size</t>
-  </si>
-  <si>
-    <t>NVDLA_PDP_RECIP_KERNEL_HEIGHT (0-16) = 2^16 / pool_size</t>
-  </si>
-  <si>
     <t>NVDLA_PDP_PAD_LEFT (0-2) = padding[1], 
 NVDLA_PDP_PAD_TOP (4-6) = padding[0], 
 NVDLA_PDP_PAD_RIGHT (8-10) = padding[1] , 
@@ -5665,16 +5649,10 @@
     <t>NVDLA_CDP_DATIN_OFFSET (0-15) = 0</t>
   </si>
   <si>
-    <t>NVDLA_CDP_DATIN_SCALE (0-15) = 0</t>
-  </si>
-  <si>
     <t>NVDLA_CDP_DATIN_SHIFTER (0-4) = 0</t>
   </si>
   <si>
     <t>NVDLA_CDP_DATOUT_OFFSET (0-31) = 0</t>
-  </si>
-  <si>
-    <t>NVDLA_CDP_DATOUT_SCALE (0-15) = 0</t>
   </si>
   <si>
     <t>NVDLA_CDP_DATOUT_SHIFTER (0-5) = 0</t>
@@ -5708,18 +5686,6 @@
 For sigm/tanh:   LE/ Table X =linear for dense (65), LO/ Table Y=linear for raw (257)</t>
   </si>
   <si>
-    <t>NVDLA_CDP_LUT_LE_INDEX_OFFSET (0-7) = 0
-(ie X[0] =f(2^0) and scale in = 0), 
-NVDLA_CDP_LUT_LE_INDEX_SELECT (8-15) = 0 (unused), 
-NVDLA_CDP_LUT_LO_INDEX_SELECT (16-23) = -M = 14
-(We want SF_lut = 257-1/((max-min) * SF_in ≈ 2^M
-max = 5,000,000, min = 0 (squares can't go under 0)
-SF_in = 0 so SF_lut ≈ 5e-5 ≈ 2^-14 ≈ 6e-5 ... max ≈ 4.2m)</t>
-  </si>
-  <si>
-    <t>NVDLA_CDP_LUT_LO_END_LOW (0-31) = 2^22 = 4194304</t>
-  </si>
-  <si>
     <t>NVDLA_CDP_LUT_LO_START_LOW (0-31) = low_bits(O_lut) = 0</t>
   </si>
   <si>
@@ -5727,39 +5693,6 @@
   </si>
   <si>
     <t>NVDLA_CDP_LUT_LO_END_HIGH (0-5) = 0</t>
-  </si>
-  <si>
-    <t>NVDLA_CDP_LUT_LE_START_LOW (0-31) = 0 (unused)</t>
-  </si>
-  <si>
-    <t>NVDLA_CDP_LUT_LE_START_HIGH (0-5) = 0 (unused)</t>
-  </si>
-  <si>
-    <t>NVDLA_CDP_LUT_LE_END_LOW (0-31) = 0 (unused)</t>
-  </si>
-  <si>
-    <t>NVDLA_CDP_LUT_LE_END_HIGH (0-5) = 0 (unused)</t>
-  </si>
-  <si>
-    <t>NVDLA_CDP_LUT_LE_SLOPE_UFLOW_SHIFT (0-4) = 0, 
-NVDLA_CDP_LUT_LE_SLOPE_OFLOW_SHIFT (5-9) = 0</t>
-  </si>
-  <si>
-    <t>NVDLA_CDP_LUT_LE_SLOPE_UFLOW_SCALE (0-15) = 0 (unused as 
-input never less than 0 and range of linear table Y covers this), 
-NVDLA_CDP_LUT_LE_SLOPE_OFLOW_SCALE (16-31) =  0 (unused as
-Table Y covers a larger range)</t>
-  </si>
-  <si>
-    <t>NVDLA_CDP_LUT_LO_SLOPE_UFLOW_SCALE (0-15) = 0 (unused
-as smaller values provided by Table X), 
-NVDLA_CDP_LUT_LO_SLOPE_OFLOW_SCALE (16-31) = 2^-M * 
-dy/dx((b + alpha/n * x)^-beta) = (b+alpha/n*x)^(-beta-1) * x * 
--beta*alpha/n* 2^14</t>
-  </si>
-  <si>
-    <t>NVDLA_CDP_LUT_LO_SLOPE_UFLOW_SHIFT (0-4) = 0, 
-NVDLA_CDP_LUT_LO_SLOPE_OFLOW_SHIFT (5-9) = 0</t>
   </si>
   <si>
     <t>NVDLA_CDP_DMA_EN (0) = 0,
@@ -5848,16 +5781,6 @@
 NVDLA_SDP_BS_MUL_SHIFT_VALUE (8-15) = 0</t>
   </si>
   <si>
-    <t>NVDLA_CDP_LUT_LE_FUNCTION (0) = 0 (set if 
-LE/Table X = exp or linear, LO/ Table Y = linear only so don't set), 
-NVDLA_CDP_LUT_UFLOW_PRIORITY (4) = 0 (want LE for raw 
-as should be near 0 and LE has largest range), 
-NVDLA_CDP_LUT_OFLOW_PRIORITY (5) = 0 
-(want raw again as large range), 
-NVDLA_CDP_LUT_HYBRID_PRIORITY (6) = 0 (unused as never a 
-case that one table overflows and other underflows)</t>
-  </si>
-  <si>
     <t>Relay IR Operator</t>
   </si>
   <si>
@@ -6029,6 +5952,84 @@
     <t>NVDLA_SDP_LUT_LE_INDEX_OFFSET (0-7) = 0 (unused), 
 NVDLA_SDP_LUT_LE_INDEX_SELECT (8-15) = 0 (unused), 
 NVDLA_SDP_LUT_LO_INDEX_SELECT (16-23) = 0(unused)</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_DATIN_SCALE (0-15) = 1</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_DATOUT_SCALE (0-15) = 1</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LO_END_LOW (0-31) = 2^20 = 1048576</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LE_END_LOW (0-31) = 0</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LE_END_HIGH (0-5) = 2^5</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LE_START_HIGH (0-5) = 0</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LE_START_LOW (0-31) = 0</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LE_FUNCTION (0) = 0 (set if 
+LE/Table X = exp or linear, LO/ Table Y = linear only so don't set), 
+NVDLA_CDP_LUT_UFLOW_PRIORITY (4) = 0 (unused as won't
+go under min(table Y)=0 ), 
+NVDLA_CDP_LUT_OFLOW_PRIORITY (5) = 0 
+(again unused as raw goes up to max of int range), 
+NVDLA_CDP_LUT_HYBRID_PRIORITY (6) = 0 (unused as never a 
+case that one table overflows and other underflows)</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LE_SLOPE_UFLOW_SHIFT (0-4) = 0 
+(unused see above), 
+NVDLA_CDP_LUT_LE_SLOPE_OFLOW_SHIFT (5-9) = 0 
+(unused see above))</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LO_SLOPE_UFLOW_SCALE (0-15) = 0 
+(unused as negative is impossible), 
+NVDLA_CDP_LUT_LO_SLOPE_OFLOW_SCALE (16-31) = 0 
+(unused see above)</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LO_SLOPE_UFLOW_SHIFT (0-4) = 0 (unused), 
+NVDLA_CDP_LUT_LO_SLOPE_OFLOW_SHIFT (5-9) = 0 (unused)</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LE_INDEX_OFFSET (0-7) = 0
+(ie X[0] =f(2^0) and scale in = 0), 
+NVDLA_CDP_LUT_LE_INDEX_SELECT (8-15) = 0 (unused), 
+NVDLA_CDP_LUT_LO_INDEX_SELECT (16-23) = -M = 12</t>
+  </si>
+  <si>
+    <t>NVDLA_CDP_LUT_LE_SLOPE_UFLOW_SCALE (0-15) = 0 (unused as 
+input never less than 0 and range of linear table Y covers 0-1), 
+NVDLA_CDP_LUT_LE_SLOPE_OFLOW_SCALE (16-31) =  0 (unused 
+as Table X covers full int16 range)</t>
+  </si>
+  <si>
+    <t>NVDLA_PDP_KERNEL_WIDTH (0-3) = pool_size[1], 
+NVDLA_PDP_KERNEL_HEIGHT (8-11) = pool_size[0], 
+NVDLA_PDP_KERNEL_STRIDE_WIDTH (16-19) = strides[1], 
+NVDLA_PDP_KERNEL_STRIDE_HEIGHT (20-23) = strides[0]</t>
+  </si>
+  <si>
+    <t>NVDLA_PDP_RDMA_KERNEL_WIDTH (0-3) = pooling_size[1] (from c++ driver), 
+NVDLA_PDP_RDMA_KERNEL_STRIDE_WIDTH (4-7) = strides[1]</t>
+  </si>
+  <si>
+    <t>NVDLA_PDP_RECIP_KERNEL_WIDTH (0-16) = 2^16 / pool_size[1]</t>
+  </si>
+  <si>
+    <t>NVDLA_PDP_RECIP_KERNEL_HEIGHT (0-16) = 2^16 / pool_size[0]</t>
+  </si>
+  <si>
+    <t>NVDLA_SDP_RDMA_D_OP_ENABLE (0)</t>
   </si>
 </sst>
 </file>
@@ -6627,8 +6628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C180" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E192" sqref="E192"/>
+    <sheetView tabSelected="1" topLeftCell="B376" zoomScale="94" workbookViewId="0">
+      <selection activeCell="F411" sqref="F411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9156,7 +9157,7 @@
         <v>177</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>1931</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -9511,7 +9512,9 @@
       <c r="E147" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="F147" s="9"/>
+      <c r="F147" s="9" t="s">
+        <v>1933</v>
+      </c>
     </row>
     <row r="148" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="8" t="s">
@@ -12143,7 +12146,7 @@
         <v>1178</v>
       </c>
       <c r="E281" s="3" t="s">
-        <v>1785</v>
+        <v>1781</v>
       </c>
       <c r="F281" s="9" t="s">
         <v>1179</v>
@@ -12163,7 +12166,7 @@
         <v>1182</v>
       </c>
       <c r="E282" s="3" t="s">
-        <v>1779</v>
+        <v>1775</v>
       </c>
       <c r="F282" s="9" t="s">
         <v>1183</v>
@@ -12183,7 +12186,7 @@
         <v>1186</v>
       </c>
       <c r="E283" s="3" t="s">
-        <v>1780</v>
+        <v>1776</v>
       </c>
       <c r="F283" s="9" t="s">
         <v>1187</v>
@@ -12203,7 +12206,7 @@
         <v>1190</v>
       </c>
       <c r="E284" s="3" t="s">
-        <v>1781</v>
+        <v>1777</v>
       </c>
       <c r="F284" s="9" t="s">
         <v>1191</v>
@@ -12223,7 +12226,7 @@
         <v>1194</v>
       </c>
       <c r="E285" s="3" t="s">
-        <v>1782</v>
+        <v>1778</v>
       </c>
       <c r="F285" s="9" t="s">
         <v>1195</v>
@@ -12243,7 +12246,7 @@
         <v>1198</v>
       </c>
       <c r="E286" s="3" t="s">
-        <v>1783</v>
+        <v>1779</v>
       </c>
       <c r="F286" s="9" t="s">
         <v>1199</v>
@@ -12263,7 +12266,7 @@
         <v>1202</v>
       </c>
       <c r="E287" s="3" t="s">
-        <v>1784</v>
+        <v>1780</v>
       </c>
       <c r="F287" s="9" t="s">
         <v>1203</v>
@@ -12501,7 +12504,7 @@
         <v>1244</v>
       </c>
       <c r="E299" s="3" t="s">
-        <v>1796</v>
+        <v>1792</v>
       </c>
       <c r="F299" s="9"/>
     </row>
@@ -12519,7 +12522,7 @@
         <v>1247</v>
       </c>
       <c r="E300" s="3" t="s">
-        <v>1797</v>
+        <v>1793</v>
       </c>
       <c r="F300" s="9"/>
     </row>
@@ -12796,7 +12799,7 @@
         <v>1290</v>
       </c>
       <c r="F314" s="9" t="s">
-        <v>1807</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="315" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -12816,7 +12819,7 @@
         <v>1089</v>
       </c>
       <c r="F315" s="9" t="s">
-        <v>1808</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="316" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -12952,7 +12955,7 @@
         <v>773</v>
       </c>
       <c r="F322" s="9" t="s">
-        <v>1821</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="323" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -13392,7 +13395,7 @@
         <v>1290</v>
       </c>
       <c r="F344" s="9" t="s">
-        <v>1820</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="345" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -13589,7 +13592,7 @@
         <v>1438</v>
       </c>
       <c r="E354" s="3" t="s">
-        <v>1830</v>
+        <v>1824</v>
       </c>
       <c r="F354" s="9"/>
     </row>
@@ -13607,7 +13610,7 @@
         <v>1440</v>
       </c>
       <c r="E355" s="3" t="s">
-        <v>1831</v>
+        <v>1825</v>
       </c>
       <c r="F355" s="9"/>
     </row>
@@ -13625,7 +13628,7 @@
         <v>1442</v>
       </c>
       <c r="E356" s="3" t="s">
-        <v>1832</v>
+        <v>1826</v>
       </c>
       <c r="F356" s="9"/>
     </row>
@@ -13643,7 +13646,7 @@
         <v>1444</v>
       </c>
       <c r="E357" s="3" t="s">
-        <v>1833</v>
+        <v>1827</v>
       </c>
       <c r="F357" s="9"/>
     </row>
@@ -14279,7 +14282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA87D8E-35BF-6445-9953-D74617F54FAC}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -14668,13 +14671,13 @@
         <v>318</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>1925</v>
+        <v>1908</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>322</v>
       </c>
@@ -15412,8 +15415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAEFD91-A0A0-3841-ACA7-980790F4A95E}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A29" zoomScale="93" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15563,7 +15566,7 @@
         <v>649</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>1924</v>
+        <v>1907</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>1566</v>
@@ -15885,7 +15888,7 @@
         <v>781</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1932</v>
+        <v>1915</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>782</v>
@@ -16054,7 +16057,7 @@
         <v>837</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>1926</v>
+        <v>1909</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>838</v>
@@ -16124,7 +16127,7 @@
         <v>862</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>1871</v>
+        <v>1855</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>863</v>
@@ -16138,7 +16141,7 @@
         <v>867</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>1872</v>
+        <v>1856</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>868</v>
@@ -16152,7 +16155,7 @@
         <v>872</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>1874</v>
+        <v>1858</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>873</v>
@@ -16166,7 +16169,7 @@
         <v>877</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>1873</v>
+        <v>1857</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>878</v>
@@ -16532,8 +16535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D171253D-D4FA-5E47-BC95-CB03F8C605CA}">
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A33" zoomScale="119" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16724,7 +16727,7 @@
         <v>1093</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1768</v>
+        <v>1930</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>1094</v>
@@ -16920,7 +16923,7 @@
         <v>1161</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>1767</v>
+        <v>1929</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>1094</v>
@@ -16934,7 +16937,7 @@
         <v>1165</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>1769</v>
+        <v>1931</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>1166</v>
@@ -16948,7 +16951,7 @@
         <v>1170</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1770</v>
+        <v>1932</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>1171</v>
@@ -16962,7 +16965,7 @@
         <v>1174</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1771</v>
+        <v>1767</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>389</v>
@@ -16976,10 +16979,10 @@
         <v>1178</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1772</v>
+        <v>1768</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>1785</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -16990,10 +16993,10 @@
         <v>1182</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1773</v>
+        <v>1769</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>1779</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -17004,10 +17007,10 @@
         <v>1186</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1774</v>
+        <v>1770</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>1780</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -17018,10 +17021,10 @@
         <v>1190</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1775</v>
+        <v>1771</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>1781</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -17032,10 +17035,10 @@
         <v>1194</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1776</v>
+        <v>1772</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>1782</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -17046,10 +17049,10 @@
         <v>1198</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>1777</v>
+        <v>1773</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>1783</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -17060,10 +17063,10 @@
         <v>1202</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1778</v>
+        <v>1774</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>1784</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -17074,7 +17077,7 @@
         <v>1205</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1786</v>
+        <v>1782</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>234</v>
@@ -17088,7 +17091,7 @@
         <v>1208</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1787</v>
+        <v>1783</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>229</v>
@@ -17102,7 +17105,7 @@
         <v>1211</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>1788</v>
+        <v>1784</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>249</v>
@@ -17116,7 +17119,7 @@
         <v>1214</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>1789</v>
+        <v>1785</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>259</v>
@@ -17130,7 +17133,7 @@
         <v>1217</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>1927</v>
+        <v>1910</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>838</v>
@@ -17144,7 +17147,7 @@
         <v>1220</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>1790</v>
+        <v>1786</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>843</v>
@@ -17158,7 +17161,7 @@
         <v>1223</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>1792</v>
+        <v>1788</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>585</v>
@@ -17172,7 +17175,7 @@
         <v>1226</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>1791</v>
+        <v>1787</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>1227</v>
@@ -17186,7 +17189,7 @@
         <v>1231</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>1793</v>
+        <v>1789</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>1232</v>
@@ -17200,7 +17203,7 @@
         <v>1235</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>1794</v>
+        <v>1790</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>1236</v>
@@ -17214,7 +17217,7 @@
         <v>1249</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>1795</v>
+        <v>1791</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>1250</v>
@@ -17330,8 +17333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C729E8E-747C-6746-842B-1F6502A00978}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A15" zoomScale="109" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17368,7 +17371,7 @@
         <v>1264</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1798</v>
+        <v>1794</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>1049</v>
@@ -17382,7 +17385,7 @@
         <v>1267</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1799</v>
+        <v>1795</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1054</v>
@@ -17396,7 +17399,7 @@
         <v>1270</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1800</v>
+        <v>1796</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1059</v>
@@ -17410,7 +17413,7 @@
         <v>1273</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1801</v>
+        <v>1797</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>234</v>
@@ -17424,7 +17427,7 @@
         <v>1276</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1802</v>
+        <v>1798</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>229</v>
@@ -17438,7 +17441,7 @@
         <v>1279</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1803</v>
+        <v>1799</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>249</v>
@@ -17452,7 +17455,7 @@
         <v>1282</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1815</v>
+        <v>1811</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>259</v>
@@ -17466,7 +17469,7 @@
         <v>1285</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1804</v>
+        <v>1800</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>730</v>
@@ -17480,7 +17483,7 @@
         <v>1289</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1805</v>
+        <v>1801</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>1290</v>
@@ -17494,10 +17497,10 @@
         <v>1293</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1809</v>
+        <v>1805</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1806</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -17508,7 +17511,7 @@
         <v>1295</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1810</v>
+        <v>1806</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>1084</v>
@@ -17522,7 +17525,7 @@
         <v>1298</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1811</v>
+        <v>1807</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>742</v>
@@ -17536,10 +17539,10 @@
         <v>1309</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>1834</v>
+        <v>1828</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1835</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -17550,7 +17553,7 @@
         <v>1312</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1836</v>
+        <v>1830</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>773</v>
@@ -17564,13 +17567,13 @@
         <v>1314</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>1875</v>
+        <v>1923</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1316</v>
       </c>
@@ -17578,7 +17581,7 @@
         <v>1317</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1838</v>
+        <v>1927</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>782</v>
@@ -17592,7 +17595,7 @@
         <v>1321</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1843</v>
+        <v>1922</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>1322</v>
@@ -17606,7 +17609,7 @@
         <v>1326</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1844</v>
+        <v>1921</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>1327</v>
@@ -17620,7 +17623,7 @@
         <v>1331</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1845</v>
+        <v>1919</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>1332</v>
@@ -17634,7 +17637,7 @@
         <v>1336</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1846</v>
+        <v>1920</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>1337</v>
@@ -17648,7 +17651,7 @@
         <v>1341</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1840</v>
+        <v>1832</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>1342</v>
@@ -17662,7 +17665,7 @@
         <v>1346</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1841</v>
+        <v>1833</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>1347</v>
@@ -17676,7 +17679,7 @@
         <v>1351</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1839</v>
+        <v>1918</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>1352</v>
@@ -17690,13 +17693,13 @@
         <v>1356</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>1842</v>
+        <v>1834</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>1357</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1359</v>
       </c>
@@ -17704,13 +17707,13 @@
         <v>1360</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>1848</v>
+        <v>1928</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1362</v>
       </c>
@@ -17718,13 +17721,13 @@
         <v>1363</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>1847</v>
+        <v>1924</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1365</v>
       </c>
@@ -17732,7 +17735,7 @@
         <v>1366</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>1849</v>
+        <v>1925</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>817</v>
@@ -17746,7 +17749,7 @@
         <v>1369</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1850</v>
+        <v>1926</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>822</v>
@@ -17760,7 +17763,7 @@
         <v>1375</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1812</v>
+        <v>1808</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>1376</v>
@@ -17774,7 +17777,7 @@
         <v>1379</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1928</v>
+        <v>1911</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>838</v>
@@ -17788,7 +17791,7 @@
         <v>1382</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1813</v>
+        <v>1809</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>843</v>
@@ -17802,7 +17805,7 @@
         <v>1385</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1814</v>
+        <v>1810</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>585</v>
@@ -17816,7 +17819,7 @@
         <v>1388</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1816</v>
+        <v>1812</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>1227</v>
@@ -17830,7 +17833,7 @@
         <v>1391</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1817</v>
+        <v>1813</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>1392</v>
@@ -17844,7 +17847,7 @@
         <v>1396</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>1818</v>
+        <v>1814</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>1290</v>
@@ -17858,7 +17861,7 @@
         <v>1398</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1819</v>
+        <v>1815</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>1236</v>
@@ -17872,7 +17875,7 @@
         <v>1401</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1822</v>
+        <v>1818</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>1149</v>
@@ -17886,7 +17889,7 @@
         <v>1405</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1823</v>
+        <v>1819</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>1568</v>
@@ -17900,7 +17903,7 @@
         <v>1409</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>1824</v>
+        <v>1820</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>1410</v>
@@ -17914,7 +17917,7 @@
         <v>1414</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>1825</v>
+        <v>1916</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>1415</v>
@@ -17928,7 +17931,7 @@
         <v>1419</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>1826</v>
+        <v>1821</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>1420</v>
@@ -17942,7 +17945,7 @@
         <v>1424</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>1827</v>
+        <v>1822</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>1425</v>
@@ -17956,7 +17959,7 @@
         <v>1429</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>1828</v>
+        <v>1917</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>1430</v>
@@ -17970,7 +17973,7 @@
         <v>1434</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>1829</v>
+        <v>1823</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>1435</v>
@@ -17984,7 +17987,7 @@
         <v>1446</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>1851</v>
+        <v>1835</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>742</v>
@@ -18061,7 +18064,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18098,7 +18101,7 @@
         <v>1473</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1852</v>
+        <v>1836</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>1474</v>
@@ -18112,7 +18115,7 @@
         <v>1477</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1853</v>
+        <v>1837</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1478</v>
@@ -18126,7 +18129,7 @@
         <v>1481</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1854</v>
+        <v>1838</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1482</v>
@@ -18140,7 +18143,7 @@
         <v>1485</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1855</v>
+        <v>1839</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>1059</v>
@@ -18154,7 +18157,7 @@
         <v>1489</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1856</v>
+        <v>1840</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>229</v>
@@ -18168,7 +18171,7 @@
         <v>1493</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1857</v>
+        <v>1841</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>234</v>
@@ -18182,7 +18185,7 @@
         <v>1497</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1858</v>
+        <v>1842</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>1498</v>
@@ -18196,7 +18199,7 @@
         <v>1502</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1859</v>
+        <v>1843</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>1503</v>
@@ -18210,7 +18213,7 @@
         <v>1507</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1867</v>
+        <v>1851</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>1508</v>
@@ -18224,7 +18227,7 @@
         <v>1512</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1860</v>
+        <v>1844</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>1513</v>
@@ -18238,7 +18241,7 @@
         <v>1516</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1861</v>
+        <v>1845</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>1142</v>
@@ -18252,7 +18255,7 @@
         <v>1520</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1862</v>
+        <v>1846</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>843</v>
@@ -18266,7 +18269,7 @@
         <v>1524</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1929</v>
+        <v>1912</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>838</v>
@@ -18280,7 +18283,7 @@
         <v>1528</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1863</v>
+        <v>1847</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>848</v>
@@ -18294,7 +18297,7 @@
         <v>1532</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>1864</v>
+        <v>1848</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>1533</v>
@@ -18308,7 +18311,7 @@
         <v>1537</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1865</v>
+        <v>1849</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>1538</v>
@@ -18322,7 +18325,7 @@
         <v>1542</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1866</v>
+        <v>1850</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>853</v>
@@ -18336,7 +18339,7 @@
         <v>1546</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1868</v>
+        <v>1852</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>1547</v>
@@ -18350,7 +18353,7 @@
         <v>1551</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1869</v>
+        <v>1853</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>1552</v>
@@ -18364,7 +18367,7 @@
         <v>1555</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1870</v>
+        <v>1854</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>742</v>
@@ -18553,29 +18556,29 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>1912</v>
+        <v>1895</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>1913</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
-        <v>1876</v>
+        <v>1859</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>1877</v>
+        <v>1860</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1878</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
-        <v>1879</v>
+        <v>1862</v>
       </c>
       <c r="C4" t="s">
-        <v>1880</v>
+        <v>1863</v>
       </c>
       <c r="D4" s="28">
         <v>1</v>
@@ -18583,10 +18586,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
-        <v>1882</v>
+        <v>1865</v>
       </c>
       <c r="C5" t="s">
-        <v>1881</v>
+        <v>1864</v>
       </c>
       <c r="D5" s="28">
         <v>1</v>
@@ -18594,10 +18597,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
-        <v>1884</v>
+        <v>1867</v>
       </c>
       <c r="C6" t="s">
-        <v>1883</v>
+        <v>1866</v>
       </c>
       <c r="D6" s="28">
         <v>1</v>
@@ -18605,10 +18608,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
-        <v>1886</v>
+        <v>1869</v>
       </c>
       <c r="C7" t="s">
-        <v>1885</v>
+        <v>1868</v>
       </c>
       <c r="D7" s="28">
         <v>1</v>
@@ -18616,10 +18619,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
-        <v>1887</v>
+        <v>1870</v>
       </c>
       <c r="C8" t="s">
-        <v>1888</v>
+        <v>1871</v>
       </c>
       <c r="D8" s="28">
         <v>1</v>
@@ -18627,10 +18630,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
-        <v>1890</v>
+        <v>1873</v>
       </c>
       <c r="C9" t="s">
-        <v>1889</v>
+        <v>1872</v>
       </c>
       <c r="D9" s="28">
         <v>1</v>
@@ -18638,10 +18641,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
-        <v>1893</v>
+        <v>1876</v>
       </c>
       <c r="C10" t="s">
-        <v>1891</v>
+        <v>1874</v>
       </c>
       <c r="D10" s="28">
         <v>1</v>
@@ -18649,10 +18652,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>1894</v>
+        <v>1877</v>
       </c>
       <c r="C11" t="s">
-        <v>1892</v>
+        <v>1875</v>
       </c>
       <c r="D11" s="28">
         <v>1</v>
@@ -18660,10 +18663,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
-        <v>1895</v>
+        <v>1878</v>
       </c>
       <c r="C12" t="s">
-        <v>1896</v>
+        <v>1879</v>
       </c>
       <c r="D12" s="28">
         <v>1</v>
@@ -18671,10 +18674,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>1898</v>
+        <v>1881</v>
       </c>
       <c r="C13" t="s">
-        <v>1897</v>
+        <v>1880</v>
       </c>
       <c r="D13" s="28">
         <v>1</v>
@@ -18682,35 +18685,35 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>1900</v>
+        <v>1883</v>
       </c>
       <c r="C14" t="s">
-        <v>1899</v>
+        <v>1882</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>1906</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
-        <v>1902</v>
+        <v>1885</v>
       </c>
       <c r="C15" t="s">
-        <v>1901</v>
+        <v>1884</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>1906</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
-        <v>1903</v>
+        <v>1886</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>1904</v>
+        <v>1887</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>1906</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -18718,30 +18721,30 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>1905</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="31" t="s">
-        <v>1914</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>1908</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="25" t="s">
-        <v>1876</v>
+        <v>1859</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>1907</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
-        <v>1879</v>
+        <v>1862</v>
       </c>
       <c r="C24" s="28">
         <v>1</v>
@@ -18749,7 +18752,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
-        <v>1882</v>
+        <v>1865</v>
       </c>
       <c r="C25" s="28">
         <v>1</v>
@@ -18757,7 +18760,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
-        <v>1884</v>
+        <v>1867</v>
       </c>
       <c r="C26" s="28">
         <v>1</v>
@@ -18765,7 +18768,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
-        <v>1886</v>
+        <v>1869</v>
       </c>
       <c r="C27" s="28">
         <v>1</v>
@@ -18773,7 +18776,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
-        <v>1887</v>
+        <v>1870</v>
       </c>
       <c r="C28" s="28">
         <v>1</v>
@@ -18781,7 +18784,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="8" t="s">
-        <v>1890</v>
+        <v>1873</v>
       </c>
       <c r="C29" s="28">
         <v>1</v>
@@ -18789,7 +18792,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="8" t="s">
-        <v>1893</v>
+        <v>1876</v>
       </c>
       <c r="C30" s="28">
         <v>1</v>
@@ -18797,7 +18800,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="8" t="s">
-        <v>1894</v>
+        <v>1877</v>
       </c>
       <c r="C31" s="28">
         <v>1</v>
@@ -18805,7 +18808,7 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="8" t="s">
-        <v>1895</v>
+        <v>1878</v>
       </c>
       <c r="C32" s="28">
         <v>1</v>
@@ -18813,82 +18816,82 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="8" t="s">
-        <v>1898</v>
+        <v>1881</v>
       </c>
       <c r="C33" s="28">
         <f>(12-2)/12</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="D33" t="s">
-        <v>1930</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" s="8" t="s">
-        <v>1900</v>
+        <v>1883</v>
       </c>
       <c r="C34" s="30">
         <f>6/9</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D34" t="s">
-        <v>1911</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B35" s="8" t="s">
-        <v>1902</v>
+        <v>1885</v>
       </c>
       <c r="C35" s="30">
         <f>6/8</f>
         <v>0.75</v>
       </c>
       <c r="D35" t="s">
-        <v>1910</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" s="10" t="s">
-        <v>1903</v>
+        <v>1886</v>
       </c>
       <c r="C36" s="29">
         <f>5/6</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="D36" t="s">
-        <v>1909</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>1915</v>
+        <v>1898</v>
       </c>
       <c r="B39" t="s">
-        <v>1913</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>1916</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>1917</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="33"/>
       <c r="B45" s="26" t="s">
-        <v>1920</v>
+        <v>1903</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>1921</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
-        <v>1922</v>
+        <v>1905</v>
       </c>
       <c r="B46">
         <v>65</v>
@@ -18899,7 +18902,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="34" t="s">
-        <v>1919</v>
+        <v>1902</v>
       </c>
       <c r="B47" s="11">
         <v>69</v>
@@ -18910,13 +18913,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1923</v>
+        <v>1906</v>
       </c>
       <c r="B48" t="s">
-        <v>1918</v>
+        <v>1901</v>
       </c>
       <c r="C48" t="s">
-        <v>1918</v>
+        <v>1901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>